<commit_message>
Sample Changes to file
Sample Changes
</commit_message>
<xml_diff>
--- a/Credentialing Requirement Report.xlsx
+++ b/Credentialing Requirement Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Credentialing Requirement Report</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Sample row added</t>
+  </si>
+  <si>
+    <t>Mysample</t>
   </si>
 </sst>
 </file>
@@ -593,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -745,6 +748,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>

</xml_diff>